<commit_message>
[BAF510] : 채권 중간 대비 엑셀 annotation/commenting
</commit_message>
<xml_diff>
--- a/BAF510채권/BOND_FINAL_PREP.xlsx
+++ b/BAF510채권/BOND_FINAL_PREP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chlje\VSCodeProjects\KAIST_MFE\BAF510채권\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VSCodeProjects\KAIST_MFE\BAF510채권\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CAEAE4-958D-4AA1-8C36-1ED66971457D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200D2A5C-9D17-40CB-BECC-738BA11FED6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{C3082CC5-84DE-479A-9159-2F50C75C6A87}"/>
+    <workbookView xWindow="-16320" yWindow="-6945" windowWidth="16440" windowHeight="28440" activeTab="3" xr2:uid="{C3082CC5-84DE-479A-9159-2F50C75C6A87}"/>
   </bookViews>
   <sheets>
     <sheet name="price" sheetId="1" r:id="rId1"/>
@@ -179,6 +179,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="G33" authorId="0" shapeId="0" xr:uid="{414BADAB-53DE-4BD4-BCCF-FA4DD94DD517}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jaepil Choi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+채권 현재 가격에 쿠폰율 적용해서 나온 쿠폰금액
+즉, FV말고 PV 기준 coupon</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A38" authorId="0" shapeId="0" xr:uid="{9138BCDA-0504-4E94-B7EC-95F4F9B4D504}">
       <text>
         <r>
@@ -248,6 +273,30 @@
           </rPr>
           <t xml:space="preserve">
 coupon rate &lt; current yield인 상황. bond is traded at discount</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E86" authorId="0" shapeId="0" xr:uid="{726AD0B6-15A2-40FA-96D7-4B1778A25FB1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jaepil Choi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Par 기준 weight</t>
         </r>
       </text>
     </comment>
@@ -427,7 +476,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="111">
   <si>
     <t>PV/FV calculator</t>
   </si>
@@ -716,12 +765,58 @@
   <si>
     <t xml:space="preserve">total return </t>
   </si>
+  <si>
+    <t>DV01</t>
+  </si>
+  <si>
+    <t>Modified Duration</t>
+  </si>
+  <si>
+    <t>principal</t>
+  </si>
+  <si>
+    <t>per period</t>
+  </si>
+  <si>
+    <t>periods</t>
+  </si>
+  <si>
+    <t>dollar coupon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">price </t>
+  </si>
+  <si>
+    <t>duration in periods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">그냥 이 부분은 T2 &gt; volatility 참고. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">아래와 같이 closed form solution을 함수화 시킨 것. </t>
+  </si>
+  <si>
+    <t>zero coupon bond</t>
+  </si>
+  <si>
+    <t>modified duration</t>
+  </si>
+  <si>
+    <t>macaulay duration</t>
+  </si>
+  <si>
+    <t>First Order Approximation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">엑셀에 있음. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
@@ -863,7 +958,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -891,6 +986,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6783,10 +6879,103 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>538369</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>8283</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>416041</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>120342</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98C5EF6C-F639-6F5F-DE22-FBA1B46502B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3627782" y="2774674"/>
+          <a:ext cx="3538585" cy="2588559"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>488674</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>91931</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>546653</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>39289</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D944455C-00FF-911F-C94F-804D474381EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3578087" y="5525322"/>
+          <a:ext cx="3718892" cy="1852358"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6824,7 +7013,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -6930,7 +7119,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7072,7 +7261,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7083,25 +7272,25 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -7109,7 +7298,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -7117,7 +7306,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -7125,7 +7314,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -7134,7 +7323,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
@@ -7148,7 +7337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -7165,7 +7354,7 @@
         <v>127.44293212890625</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>2</v>
       </c>
@@ -7182,7 +7371,7 @@
         <v>119.9462890625</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>3</v>
       </c>
@@ -7199,7 +7388,7 @@
         <v>112.890625</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>4</v>
       </c>
@@ -7216,82 +7405,82 @@
         <v>106.25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>20</v>
       </c>
@@ -7308,13 +7497,13 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>9</v>
       </c>
@@ -7327,28 +7516,28 @@
         <v>1566.5298461914063</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>14</v>
       </c>
@@ -7363,7 +7552,7 @@
         <v>885.30078781434736</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
         <v>15</v>
       </c>
@@ -7378,7 +7567,7 @@
         <v>849.53703128475104</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>16</v>
       </c>
@@ -7392,7 +7581,7 @@
         <v>850.509253161836</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>17</v>
       </c>
@@ -7406,7 +7595,7 @@
         <v>851.53980835154618</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>18</v>
       </c>
@@ -7420,7 +7609,7 @@
         <v>852.63219685263891</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D44" s="3">
         <v>18</v>
       </c>
@@ -7428,7 +7617,7 @@
         <v>853.7901286637973</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>19</v>
       </c>
@@ -7443,7 +7632,7 @@
         <v>855.01753638362493</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>20</v>
       </c>
@@ -7458,7 +7647,7 @@
         <v>856.31858856664269</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>21</v>
       </c>
@@ -7473,7 +7662,7 @@
         <v>857.69770388064126</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>22</v>
       </c>
@@ -7488,7 +7677,7 @@
         <v>859.15956611347974</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>23</v>
       </c>
@@ -7503,7 +7692,7 @@
         <v>860.70914008028842</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>25</v>
       </c>
@@ -7518,7 +7707,7 @@
         <v>862.35168848510557</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D51" s="3">
         <v>14.5</v>
       </c>
@@ -7526,7 +7715,7 @@
         <v>864.09278979421219</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D52" s="3">
         <v>14</v>
       </c>
@@ -7534,7 +7723,7 @@
         <v>865.93835718186483</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D53" s="3">
         <v>13.5</v>
       </c>
@@ -7542,7 +7731,7 @@
         <v>867.89465861277665</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D54" s="3">
         <v>13</v>
       </c>
@@ -7550,7 +7739,7 @@
         <v>869.96833812954333</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D55" s="3">
         <v>12.5</v>
       </c>
@@ -7558,7 +7747,7 @@
         <v>872.16643841731593</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D56" s="3">
         <v>12</v>
       </c>
@@ -7566,7 +7755,7 @@
         <v>874.49642472235485</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D57" s="3">
         <v>11.5</v>
       </c>
@@ -7574,7 +7763,7 @@
         <v>876.96621020569614</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D58" s="3">
         <v>11</v>
       </c>
@@ -7582,7 +7771,7 @@
         <v>879.58418281803779</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D59" s="3">
         <v>10.5</v>
       </c>
@@ -7590,7 +7779,7 @@
         <v>882.35923378712016</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D60" s="3">
         <v>10</v>
       </c>
@@ -7598,7 +7787,7 @@
         <v>885.30078781434736</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D61" s="3">
         <v>9.5</v>
       </c>
@@ -7606,7 +7795,7 @@
         <v>888.41883508320825</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D62" s="3">
         <v>9</v>
       </c>
@@ -7614,7 +7803,7 @@
         <v>891.72396518820074</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D63" s="3">
         <v>8.5</v>
       </c>
@@ -7622,7 +7811,7 @@
         <v>895.22740309949268</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D64" s="3">
         <v>8</v>
       </c>
@@ -7630,7 +7819,7 @@
         <v>898.94104728546222</v>
       </c>
     </row>
-    <row r="65" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D65" s="3">
         <v>7.5</v>
       </c>
@@ -7638,7 +7827,7 @@
         <v>902.87751012259014</v>
       </c>
     </row>
-    <row r="66" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D66" s="3">
         <v>7</v>
       </c>
@@ -7646,7 +7835,7 @@
         <v>907.05016072994545</v>
       </c>
     </row>
-    <row r="67" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D67" s="3">
         <v>6.5</v>
       </c>
@@ -7654,7 +7843,7 @@
         <v>911.47317037374228</v>
       </c>
     </row>
-    <row r="68" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D68" s="3">
         <v>6</v>
       </c>
@@ -7662,7 +7851,7 @@
         <v>916.16156059616674</v>
       </c>
     </row>
-    <row r="69" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D69" s="3">
         <v>5.5</v>
       </c>
@@ -7670,7 +7859,7 @@
         <v>921.13125423193674</v>
       </c>
     </row>
-    <row r="70" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D70" s="3">
         <v>5</v>
       </c>
@@ -7678,7 +7867,7 @@
         <v>926.39912948585288</v>
       </c>
     </row>
-    <row r="71" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D71" s="3">
         <v>4.5</v>
       </c>
@@ -7686,7 +7875,7 @@
         <v>931.98307725500422</v>
       </c>
     </row>
-    <row r="72" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D72" s="3">
         <v>4</v>
       </c>
@@ -7694,7 +7883,7 @@
         <v>937.90206189030448</v>
       </c>
     </row>
-    <row r="73" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D73" s="3">
         <v>3.5</v>
       </c>
@@ -7702,7 +7891,7 @@
         <v>944.17618560372273</v>
       </c>
     </row>
-    <row r="74" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D74" s="3">
         <v>3</v>
       </c>
@@ -7710,7 +7899,7 @@
         <v>950.82675673994606</v>
       </c>
     </row>
-    <row r="75" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D75" s="3">
         <v>2.5</v>
       </c>
@@ -7718,7 +7907,7 @@
         <v>957.87636214434281</v>
       </c>
     </row>
-    <row r="76" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D76" s="3">
         <v>2</v>
       </c>
@@ -7726,7 +7915,7 @@
         <v>965.34894387300346</v>
       </c>
     </row>
-    <row r="77" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D77" s="3">
         <v>1.5</v>
       </c>
@@ -7734,7 +7923,7 @@
         <v>973.26988050538364</v>
       </c>
     </row>
-    <row r="78" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D78" s="3">
         <v>1</v>
       </c>
@@ -7742,7 +7931,7 @@
         <v>981.66607333570664</v>
       </c>
     </row>
-    <row r="79" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D79" s="3">
         <v>0.5</v>
       </c>
@@ -7750,7 +7939,7 @@
         <v>990.56603773584902</v>
       </c>
     </row>
-    <row r="80" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D80" s="3">
         <v>0</v>
       </c>
@@ -7758,22 +7947,22 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>14</v>
       </c>
@@ -7788,7 +7977,7 @@
         <v>1150.8261172101793</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
         <v>15</v>
       </c>
@@ -7803,7 +7992,7 @@
         <v>1220.9983991771542</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>16</v>
       </c>
@@ -7817,7 +8006,7 @@
         <v>1218.6173367450629</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>17</v>
       </c>
@@ -7831,7 +8020,7 @@
         <v>1216.1434128781204</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>18</v>
       </c>
@@ -7845,7 +8034,7 @@
         <v>1213.573005980367</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D91" s="3">
         <v>18</v>
       </c>
@@ -7853,7 +8042,7 @@
         <v>1210.9023532136014</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>19</v>
       </c>
@@ -7868,7 +8057,7 @@
         <v>1208.127544988932</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>20</v>
       </c>
@@ -7883,7 +8072,7 @@
         <v>1205.2445192435002</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>21</v>
       </c>
@@ -7898,7 +8087,7 @@
         <v>1202.2490554939968</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>22</v>
       </c>
@@ -7913,7 +8102,7 @@
         <v>1199.1367686582626</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>23</v>
       </c>
@@ -7928,7 +8117,7 @@
         <v>1195.9031026359348</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>25</v>
       </c>
@@ -7943,7 +8132,7 @@
         <v>1192.5433236387362</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D98" s="3">
         <v>14.5</v>
       </c>
@@ -7951,7 +8140,7 @@
         <v>1189.0525132606472</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D99" s="3">
         <v>14</v>
       </c>
@@ -7959,7 +8148,7 @@
         <v>1185.4255612778124</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D100" s="3">
         <v>13.5</v>
       </c>
@@ -7967,7 +8156,7 @@
         <v>1181.6571581676471</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D101" s="3">
         <v>13</v>
       </c>
@@ -7975,7 +8164,7 @@
         <v>1177.7417873361853</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D102" s="3">
         <v>12.5</v>
       </c>
@@ -7983,7 +8172,7 @@
         <v>1173.6737170422964</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D103" s="3">
         <v>12</v>
       </c>
@@ -7991,7 +8180,7 @@
         <v>1169.4469920069462</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D104" s="3">
         <v>11.5</v>
       </c>
@@ -7999,7 +8188,7 @@
         <v>1165.055424695217</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D105" s="3">
         <v>11</v>
       </c>
@@ -8007,7 +8196,7 @@
         <v>1160.4925862583304</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D106" s="3">
         <v>10.5</v>
       </c>
@@ -8015,7 +8204,7 @@
         <v>1155.7517971224054</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D107" s="3">
         <v>10</v>
       </c>
@@ -8023,7 +8212,7 @@
         <v>1150.8261172101793</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D108" s="3">
         <v>9.5</v>
       </c>
@@ -8031,7 +8220,7 @@
         <v>1145.7083357813763</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D109" s="3">
         <v>9</v>
       </c>
@@ -8039,7 +8228,7 @@
         <v>1140.3909608768499</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D110" s="3">
         <v>8.5</v>
       </c>
@@ -8047,7 +8236,7 @@
         <v>1134.8662083510471</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D111" s="3">
         <v>8</v>
       </c>
@@ -8055,7 +8244,7 @@
         <v>1129.125990476738</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D112" s="3">
         <v>7.5</v>
       </c>
@@ -8063,7 +8252,7 @@
         <v>1123.1619041053309</v>
       </c>
     </row>
-    <row r="113" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D113" s="3">
         <v>7</v>
       </c>
@@ -8071,7 +8260,7 @@
         <v>1116.9652183654387</v>
       </c>
     </row>
-    <row r="114" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D114" s="3">
         <v>6.5</v>
       </c>
@@ -8079,7 +8268,7 @@
         <v>1110.5268618816908</v>
       </c>
     </row>
-    <row r="115" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D115" s="3">
         <v>6</v>
       </c>
@@ -8087,7 +8276,7 @@
         <v>1103.8374094950768</v>
       </c>
     </row>
-    <row r="116" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D116" s="3">
         <v>5.5</v>
       </c>
@@ -8095,7 +8284,7 @@
         <v>1096.8870684653848</v>
       </c>
     </row>
-    <row r="117" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D117" s="3">
         <v>5</v>
       </c>
@@ -8103,7 +8292,7 @@
         <v>1089.6656641355348</v>
       </c>
     </row>
-    <row r="118" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D118" s="3">
         <v>4.5</v>
       </c>
@@ -8111,7 +8300,7 @@
         <v>1082.1626250368208</v>
       </c>
     </row>
-    <row r="119" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D119" s="3">
         <v>4</v>
       </c>
@@ -8119,7 +8308,7 @@
         <v>1074.366967413257</v>
       </c>
     </row>
-    <row r="120" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D120" s="3">
         <v>3.5</v>
       </c>
@@ -8127,7 +8316,7 @@
         <v>1066.2672791423738</v>
       </c>
     </row>
-    <row r="121" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D121" s="3">
         <v>3</v>
       </c>
@@ -8135,7 +8324,7 @@
         <v>1057.8517030289265</v>
       </c>
     </row>
-    <row r="122" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D122" s="3">
         <v>2.5</v>
       </c>
@@ -8143,7 +8332,7 @@
         <v>1049.1079194470547</v>
       </c>
     </row>
-    <row r="123" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D123" s="3">
         <v>2</v>
       </c>
@@ -8151,7 +8340,7 @@
         <v>1040.0231283054898</v>
       </c>
     </row>
-    <row r="124" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D124" s="3">
         <v>1.5</v>
       </c>
@@ -8159,7 +8348,7 @@
         <v>1030.5840303094039</v>
       </c>
     </row>
-    <row r="125" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D125" s="3">
         <v>1</v>
       </c>
@@ -8167,7 +8356,7 @@
         <v>1020.7768074914707</v>
       </c>
     </row>
-    <row r="126" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D126" s="3">
         <v>0.5</v>
       </c>
@@ -8175,7 +8364,7 @@
         <v>1010.5871029836381</v>
       </c>
     </row>
-    <row r="127" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D127" s="3">
         <v>0</v>
       </c>
@@ -8197,23 +8386,23 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -8221,7 +8410,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -8229,7 +8418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
@@ -8237,7 +8426,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -8245,7 +8434,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>32</v>
       </c>
@@ -8253,7 +8442,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -8262,7 +8451,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -8271,7 +8460,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -8280,7 +8469,7 @@
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -8289,7 +8478,7 @@
         <v>597.51912424641466</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>34</v>
       </c>
@@ -8298,7 +8487,7 @@
         <v>342.72896332894379</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
@@ -8307,7 +8496,7 @@
         <v>940.24808757535845</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>35</v>
       </c>
@@ -8315,7 +8504,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>36</v>
       </c>
@@ -8341,7 +8530,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>9.9</v>
       </c>
@@ -8374,7 +8563,7 @@
         <v>940.37050780850541</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <f>A18-0.1</f>
         <v>9.8000000000000007</v>
@@ -8408,7 +8597,7 @@
         <v>940.60190288853642</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <f t="shared" ref="A20:A83" si="7">A19-0.1</f>
         <v>9.7000000000000011</v>
@@ -8442,7 +8631,7 @@
         <v>940.94344600496311</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <f t="shared" si="7"/>
         <v>9.6000000000000014</v>
@@ -8476,7 +8665,7 @@
         <v>941.39632297749336</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <f t="shared" si="7"/>
         <v>9.5000000000000018</v>
@@ -8510,7 +8699,7 @@
         <v>941.96173239200323</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <f t="shared" si="7"/>
         <v>9.4000000000000021</v>
@@ -8544,7 +8733,7 @@
         <v>942.10260119547297</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <f t="shared" si="7"/>
         <v>9.3000000000000025</v>
@@ -8578,7 +8767,7 @@
         <v>942.35264345743121</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <f t="shared" si="7"/>
         <v>9.2000000000000028</v>
@@ -8612,7 +8801,7 @@
         <v>942.71303450558116</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <f t="shared" si="7"/>
         <v>9.1000000000000032</v>
@@ -8646,7 +8835,7 @@
         <v>943.18496232084101</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <f t="shared" si="7"/>
         <v>9.0000000000000036</v>
@@ -8680,7 +8869,7 @@
         <v>943.76962767356349</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <f t="shared" si="7"/>
         <v>8.9000000000000039</v>
@@ -8714,7 +8903,7 @@
         <v>943.92995971872335</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <f t="shared" si="7"/>
         <v>8.8000000000000043</v>
@@ -8748,7 +8937,7 @@
         <v>944.19967475761518</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <f t="shared" si="7"/>
         <v>8.7000000000000046</v>
@@ -8782,7 +8971,7 @@
         <v>944.57995037373348</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <f t="shared" si="7"/>
         <v>8.600000000000005</v>
@@ -8816,7 +9005,7 @@
         <v>945.07197682807259</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <f t="shared" si="7"/>
         <v>8.5000000000000053</v>
@@ -8850,7 +9039,7 @@
         <v>945.67695719560925</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <f t="shared" si="7"/>
         <v>8.4000000000000057</v>
@@ -8884,7 +9073,7 @@
         <v>945.85782296075274</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <f t="shared" si="7"/>
         <v>8.300000000000006</v>
@@ -8918,7 +9107,7 @@
         <v>946.1482927793096</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <f t="shared" si="7"/>
         <v>8.2000000000000064</v>
@@ -8952,7 +9141,7 @@
         <v>946.54954661463398</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <f t="shared" si="7"/>
         <v>8.1000000000000068</v>
@@ -8986,7 +9175,7 @@
         <v>947.06277713320196</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <f t="shared" si="7"/>
         <v>8.0000000000000071</v>
@@ -9020,7 +9209,7 @@
         <v>947.68918984136781</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <f t="shared" si="7"/>
         <v>7.9000000000000075</v>
@@ -9054,7 +9243,7 @@
         <v>947.89171868109418</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <f t="shared" si="7"/>
         <v>7.8000000000000078</v>
@@ -9088,7 +9277,7 @@
         <v>948.20408479219702</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <f t="shared" si="7"/>
         <v>7.7000000000000082</v>
@@ -9122,7 +9311,7 @@
         <v>948.62747064878431</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <f t="shared" si="7"/>
         <v>7.6000000000000085</v>
@@ -9156,7 +9345,7 @@
         <v>949.1630714551136</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <f t="shared" si="7"/>
         <v>7.5000000000000089</v>
@@ -9190,7 +9379,7 @@
         <v>949.81209528264321</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <f t="shared" si="7"/>
         <v>7.4000000000000092</v>
@@ -9224,7 +9413,7 @@
         <v>950.03747866605386</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <f t="shared" si="7"/>
         <v>7.3000000000000096</v>
@@ -9258,7 +9447,7 @@
         <v>950.37294536579316</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <f t="shared" si="7"/>
         <v>7.2000000000000099</v>
@@ -9292,7 +9481,7 @@
         <v>950.81968050481248</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <f t="shared" si="7"/>
         <v>7.1000000000000103</v>
@@ -9326,7 +9515,7 @@
         <v>951.37888196473011</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <f t="shared" si="7"/>
         <v>7.0000000000000107</v>
@@ -9360,7 +9549,7 @@
         <v>952.05176052318848</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <f t="shared" si="7"/>
         <v>6.900000000000011</v>
@@ -9394,7 +9583,7 @@
         <v>952.30125545018655</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <f t="shared" si="7"/>
         <v>6.8000000000000114</v>
@@ -9428,7 +9617,7 @@
         <v>952.66109327093704</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <f t="shared" si="7"/>
         <v>6.7000000000000117</v>
@@ -9462,7 +9651,7 @@
         <v>953.13246190292227</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <f t="shared" si="7"/>
         <v>6.6000000000000121</v>
@@ -9496,7 +9685,7 @@
         <v>953.71656205237571</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <f t="shared" si="7"/>
         <v>6.5000000000000124</v>
@@ -9530,7 +9719,7 @@
         <v>954.41460735196392</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <f t="shared" si="7"/>
         <v>6.4000000000000128</v>
@@ -9564,7 +9753,7 @@
         <v>954.68953995744619</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <f t="shared" si="7"/>
         <v>6.3000000000000131</v>
@@ -9598,7 +9787,7 @@
         <v>955.07508931086397</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <f t="shared" si="7"/>
         <v>6.2000000000000135</v>
@@ -9632,7 +9821,7 @@
         <v>955.57244627792807</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <f t="shared" si="7"/>
         <v>6.1000000000000139</v>
@@ -9666,7 +9855,7 @@
         <v>956.18281454484145</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <f t="shared" si="7"/>
         <v>6.0000000000000142</v>
@@ -9700,7 +9889,7 @@
         <v>956.90741075632184</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <f t="shared" si="7"/>
         <v>5.9000000000000146</v>
@@ -9734,7 +9923,7 @@
         <v>957.20918011260528</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <f>A58-0.1</f>
         <v>5.8000000000000149</v>
@@ -9768,7 +9957,7 @@
         <v>957.62185513298675</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <f t="shared" si="7"/>
         <v>5.7000000000000153</v>
@@ -9802,7 +9991,7 @@
         <v>958.1466297935591</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <f t="shared" si="7"/>
         <v>5.6000000000000156</v>
@@ -9836,7 +10025,7 @@
         <v>958.78471092439338</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <f t="shared" si="7"/>
         <v>5.500000000000016</v>
@@ -9870,7 +10059,7 @@
         <v>959.53731834791961</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <f t="shared" si="7"/>
         <v>5.4000000000000163</v>
@@ -9904,7 +10093,7 @@
         <v>959.86740047629837</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <f t="shared" si="7"/>
         <v>5.3000000000000167</v>
@@ -9938,7 +10127,7 @@
         <v>960.30869307532646</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <f t="shared" si="7"/>
         <v>5.2000000000000171</v>
@@ -9972,7 +10161,7 @@
         <v>960.86239340255031</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <f t="shared" si="7"/>
         <v>5.1000000000000174</v>
@@ -10006,7 +10195,7 @@
         <v>961.52971160482059</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <f t="shared" si="7"/>
         <v>5.0000000000000178</v>
@@ -10040,7 +10229,7 @@
         <v>962.31187085705506</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <f>A67-0.1</f>
         <v>4.9000000000000181</v>
@@ -10074,7 +10263,7 @@
         <v>962.67182295999442</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
         <f t="shared" si="7"/>
         <v>4.8000000000000185</v>
@@ -10108,7 +10297,7 @@
         <v>963.14330710449462</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <f t="shared" si="7"/>
         <v>4.7000000000000188</v>
@@ -10142,7 +10331,7 @@
         <v>963.72752401003561</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <f t="shared" si="7"/>
         <v>4.6000000000000192</v>
@@ -10176,7 +10365,7 @@
         <v>964.42568732267102</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <f t="shared" si="7"/>
         <v>4.5000000000000195</v>
@@ -10210,7 +10399,7 @@
         <v>965.23902375419311</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <f t="shared" si="7"/>
         <v>4.4000000000000199</v>
@@ -10244,7 +10433,7 @@
         <v>965.63048868029387</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
         <f t="shared" si="7"/>
         <v>4.3000000000000203</v>
@@ -10278,7 +10467,7 @@
         <v>966.1338249052676</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
         <f t="shared" si="7"/>
         <v>4.2000000000000206</v>
@@ -10312,7 +10501,7 @@
         <v>966.75023680093273</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
         <f t="shared" si="7"/>
         <v>4.100000000000021</v>
@@ -10346,7 +10535,7 @@
         <v>967.48094170500326</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
         <f t="shared" si="7"/>
         <v>4.0000000000000213</v>
@@ -10380,7 +10569,7 @@
         <v>968.32717006067378</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="7">
         <f t="shared" si="7"/>
         <v>3.9000000000000212</v>
@@ -10414,7 +10603,7 @@
         <v>968.75188101520951</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
         <f t="shared" si="7"/>
         <v>3.8000000000000211</v>
@@ -10448,7 +10637,7 @@
         <v>969.28882118508238</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
         <f t="shared" si="7"/>
         <v>3.700000000000021</v>
@@ -10482,7 +10671,7 @@
         <v>969.93919879532928</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
         <f t="shared" si="7"/>
         <v>3.600000000000021</v>
@@ -10516,7 +10705,7 @@
         <v>970.70423507836381</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
         <f t="shared" si="7"/>
         <v>3.5000000000000209</v>
@@ -10550,7 +10739,7 @@
         <v>971.58516441401071</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
         <f t="shared" si="7"/>
         <v>3.4000000000000208</v>
@@ -10584,7 +10773,7 @@
         <v>972.04494992854563</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="7">
         <f t="shared" ref="A84:A89" si="15">A83-0.1</f>
         <v>3.3000000000000207</v>
@@ -10618,7 +10807,7 @@
         <v>972.61734226028739</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
         <f t="shared" si="15"/>
         <v>3.2000000000000206</v>
@@ -10652,7 +10841,7 @@
         <v>973.30355369941753</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="7">
         <f t="shared" si="15"/>
         <v>3.1000000000000205</v>
@@ -10686,7 +10875,7 @@
         <v>974.1048095872593</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="7">
         <f t="shared" si="15"/>
         <v>3.0000000000000204</v>
@@ -10720,7 +10909,7 @@
         <v>975.0223484567814</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="7">
         <f t="shared" si="15"/>
         <v>2.9000000000000203</v>
@@ -10754,7 +10943,7 @@
         <v>975.5191376321153</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
         <f t="shared" si="15"/>
         <v>2.8000000000000203</v>
@@ -10788,7 +10977,7 @@
         <v>976.1289319946286</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="7">
         <f>A89-0.1</f>
         <v>2.7000000000000202</v>
@@ -10822,7 +11011,7 @@
         <v>976.85294812323082</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="7">
         <f t="shared" ref="A91:A104" si="16">A90-0.1</f>
         <v>2.6000000000000201</v>
@@ -10856,7 +11045,7 @@
         <v>977.69241569414407</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="7">
         <f t="shared" si="16"/>
         <v>2.50000000000002</v>
@@ -10890,7 +11079,7 @@
         <v>978.64857762190434</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="7">
         <f t="shared" si="16"/>
         <v>2.4000000000000199</v>
@@ -10924,7 +11113,7 @@
         <v>979.18440565938135</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="7">
         <f t="shared" si="16"/>
         <v>2.3000000000000198</v>
@@ -10958,7 +11147,7 @@
         <v>979.83365916435855</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="7">
         <f t="shared" si="16"/>
         <v>2.2000000000000197</v>
@@ -10992,7 +11181,7 @@
         <v>980.59755924035369</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
         <f t="shared" si="16"/>
         <v>2.1000000000000196</v>
@@ -11026,7 +11215,7 @@
         <v>981.4773401369074</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="7">
         <f t="shared" si="16"/>
         <v>2.0000000000000195</v>
@@ -11060,7 +11249,7 @@
         <v>982.47424939110908</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="7">
         <f t="shared" si="16"/>
         <v>1.9000000000000195</v>
@@ -11094,7 +11283,7 @@
         <v>983.05126342814685</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="7">
         <f t="shared" si="16"/>
         <v>1.8000000000000194</v>
@@ -11128,7 +11317,7 @@
         <v>983.74214632842347</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="7">
         <f t="shared" si="16"/>
         <v>1.7000000000000193</v>
@@ -11162,7 +11351,7 @@
         <v>984.54812396891816</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="7">
         <f t="shared" si="16"/>
         <v>1.6000000000000192</v>
@@ -11196,7 +11385,7 @@
         <v>985.47043542402264</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="7">
         <f t="shared" si="16"/>
         <v>1.5000000000000191</v>
@@ -11230,7 +11419,7 @@
         <v>986.51033310762011</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="7">
         <f t="shared" si="16"/>
         <v>1.400000000000019</v>
@@ -11264,7 +11453,7 @@
         <v>987.13079837419457</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="7">
         <f t="shared" si="16"/>
         <v>1.3000000000000189</v>
@@ -11298,7 +11487,7 @@
         <v>987.86560028651218</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="7">
         <f>A104-0.1</f>
         <v>1.2000000000000188</v>
@@ -11332,7 +11521,7 @@
         <v>988.71596975755381</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="7">
         <f t="shared" ref="A106:A111" si="17">A105-0.1</f>
         <v>1.1000000000000187</v>
@@ -11366,7 +11555,7 @@
         <v>989.68315095192929</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="7">
         <f t="shared" si="17"/>
         <v>1.0000000000000187</v>
@@ -11400,7 +11589,7 @@
         <v>990.76840142853928</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="7">
         <f t="shared" si="17"/>
         <v>0.90000000000001867</v>
@@ -11434,7 +11623,7 @@
         <v>991.43470774227467</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="7">
         <f t="shared" si="17"/>
         <v>0.8000000000000187</v>
@@ -11468,7 +11657,7 @@
         <v>992.21584421229556</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="7">
         <f t="shared" si="17"/>
         <v>0.70000000000001872</v>
@@ -11502,7 +11691,7 @@
         <v>993.1130470645644</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="7">
         <f t="shared" si="17"/>
         <v>0.60000000000001874</v>
@@ -11536,7 +11725,7 @@
         <v>994.12756583387068</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="7">
         <f>A111-0.1</f>
         <v>0.50000000000001876</v>
@@ -11570,7 +11759,7 @@
         <v>995.26066350710892</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="7">
         <f t="shared" ref="A113:A115" si="18">A112-0.1</f>
         <v>0.40000000000001878</v>
@@ -11604,7 +11793,7 @@
         <v>995.97533212559972</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="7">
         <f t="shared" si="18"/>
         <v>0.30000000000001881</v>
@@ -11638,7 +11827,7 @@
         <v>996.80535155399741</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="7">
         <f t="shared" si="18"/>
         <v>0.2000000000000188</v>
@@ -11672,7 +11861,7 @@
         <v>997.75196362346071</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="7">
         <f>A115-0.1</f>
         <v>0.1000000000000188</v>
@@ -11717,36 +11906,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E42AD9A-2DF5-4159-95C7-49F9F53E565B}">
   <dimension ref="A1:J165"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>42</v>
       </c>
@@ -11770,7 +11959,7 @@
         <v>2.9503507903427817E-7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -11795,7 +11984,7 @@
         <v>351.97886520637178</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -11820,7 +12009,7 @@
         <v>309.13375329129178</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -11838,7 +12027,7 @@
         <v>268.24818340515719</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -11856,7 +12045,7 @@
         <v>229.21329435243831</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>51</v>
@@ -11872,7 +12061,7 @@
         <v>191.92727772892965</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I9" s="3">
         <v>0.06</v>
       </c>
@@ -11880,7 +12069,7 @@
         <v>156.29485818418414</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I10" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -11888,7 +12077,7 @@
         <v>122.22681648916512</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I11" s="3">
         <v>0.08</v>
       </c>
@@ -11896,7 +12085,7 @@
         <v>89.63955152124106</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I12" s="3">
         <v>0.09</v>
       </c>
@@ -11904,7 +12093,7 @@
         <v>58.454677664013843</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I13" s="3">
         <v>0.1</v>
       </c>
@@ -11912,7 +12101,7 @@
         <v>28.598654463492721</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I14" s="3">
         <v>0.11</v>
       </c>
@@ -11920,7 +12109,7 @@
         <v>2.445689590672373E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I15" s="3">
         <v>0.12</v>
       </c>
@@ -11928,7 +12117,7 @@
         <v>-27.398794773011446</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I16" s="3">
         <v>0.13</v>
       </c>
@@ -11936,7 +12125,7 @@
         <v>-53.666012534235051</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I17" s="3">
         <v>0.14000000000000001</v>
       </c>
@@ -11944,7 +12133,7 @@
         <v>-78.856519916965112</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I18" s="3">
         <v>0.15</v>
       </c>
@@ -11952,7 +12141,7 @@
         <v>-103.02424269495873</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="I19" s="3">
         <v>0.16</v>
@@ -11961,7 +12150,7 @@
         <v>-126.21994808286934</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I20" s="3">
         <v>0.17</v>
       </c>
@@ -11969,7 +12158,7 @@
         <v>-148.49145555083851</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I21" s="3">
         <v>0.18</v>
       </c>
@@ -11977,7 +12166,7 @@
         <v>-169.88383189210913</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I22" s="3">
         <v>0.19</v>
       </c>
@@ -11985,7 +12174,7 @@
         <v>-190.43957184231192</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I23" s="3">
         <v>0.2</v>
       </c>
@@ -11993,32 +12182,32 @@
         <v>-210.19876543209875</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>84</v>
       </c>
       <c r="J24" s="20"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>83</v>
       </c>
       <c r="J25" s="20"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J26" s="20"/>
     </row>
-    <row r="28" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>14</v>
       </c>
@@ -12036,7 +12225,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>54</v>
       </c>
@@ -12053,7 +12242,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>56</v>
       </c>
@@ -12076,7 +12265,7 @@
         <v>-2.8171651635321676E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>55</v>
       </c>
@@ -12098,7 +12287,7 @@
         <v>-2.5315272205666643E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>16</v>
       </c>
@@ -12120,7 +12309,7 @@
         <v>-2.2548207127721442E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E36" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -12136,7 +12325,7 @@
         <v>-1.9871783648307585E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>42</v>
       </c>
@@ -12161,7 +12350,7 @@
         <v>-1.7287176559497942E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="22" cm="1">
         <f t="array" ref="A38:A67">_xlfn.SEQUENCE(B34*2, 1, 1, 1)</f>
         <v>1</v>
@@ -12189,7 +12378,7 @@
         <v>-1.479539911676056E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>2</v>
       </c>
@@ -12216,7 +12405,7 @@
         <v>-1.239729475530052E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>3</v>
       </c>
@@ -12243,7 +12432,7 @@
         <v>-1.0093529711467195E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>4</v>
       </c>
@@ -12270,7 +12459,7 @@
         <v>-7.8845866483829782E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>5</v>
       </c>
@@ -12297,7 +12486,7 @@
         <v>-5.7707593753044961E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>6</v>
       </c>
@@ -12324,7 +12513,7 @@
         <v>-3.7521487387201929E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>7</v>
       </c>
@@ -12351,7 +12540,7 @@
         <v>-1.8286597500260099E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>8</v>
       </c>
@@ -12378,7 +12567,7 @@
         <v>1.2490009027033011E-16</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>9</v>
       </c>
@@ -12405,7 +12594,7 @@
         <v>1.7343206054918764E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>10</v>
       </c>
@@ -12432,7 +12621,7 @@
         <v>3.3749887708047627E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>11</v>
       </c>
@@ -12459,7 +12648,7 @@
         <v>4.9228853962952346E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>12</v>
       </c>
@@ -12486,7 +12675,7 @@
         <v>6.3790818414415501E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>13</v>
       </c>
@@ -12513,7 +12702,7 @@
         <v>7.7448348993984922E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>14</v>
       </c>
@@ -12540,7 +12729,7 @@
         <v>9.021580533786433E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>15</v>
       </c>
@@ -12567,7 +12756,7 @@
         <v>1.0210926444320353E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>16</v>
       </c>
@@ -12594,7 +12783,7 @@
         <v>1.1314643542509925E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>17</v>
       </c>
@@ -12621,7 +12810,7 @@
         <v>1.2334656431750329E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>18</v>
       </c>
@@ -12648,7 +12837,7 @@
         <v>1.3273032997500045E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>19</v>
       </c>
@@ -12675,7 +12864,7 @@
         <v>1.4131973222634001E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>20</v>
       </c>
@@ -12702,7 +12891,7 @@
         <v>1.4913797350382202E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>21</v>
       </c>
@@ -12729,7 +12918,7 @@
         <v>1.5620933522366473E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>22</v>
       </c>
@@ -12756,7 +12945,7 @@
         <v>1.6255905022144607E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>23</v>
       </c>
@@ -12783,7 +12972,7 @@
         <v>1.6821317255353907E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>24</v>
       </c>
@@ -12810,7 +12999,7 @@
         <v>1.7319844596098199E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>25</v>
       </c>
@@ -12823,7 +13012,7 @@
         <v>14.81014462444961</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>26</v>
       </c>
@@ -12836,7 +13025,7 @@
         <v>14.309318477729091</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>27</v>
       </c>
@@ -12849,7 +13038,7 @@
         <v>13.825428480897672</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>28</v>
       </c>
@@ -12862,7 +13051,7 @@
         <v>13.357901913910794</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>29</v>
       </c>
@@ -12875,7 +13064,7 @@
         <v>12.906185424068404</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>30</v>
       </c>
@@ -12888,12 +13077,12 @@
         <v>368.74815497338295</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="3" t="s">
         <v>9</v>
@@ -12903,35 +13092,35 @@
         <v>1000.0000000000017</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>69</v>
       </c>
@@ -12939,7 +13128,7 @@
         <v>44927</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>16</v>
       </c>
@@ -12947,13 +13136,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B81" s="3"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>71</v>
       </c>
@@ -12962,7 +13151,7 @@
         <v>57259</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="19" t="s">
         <v>72</v>
       </c>
@@ -12970,7 +13159,7 @@
         <v>9.5393232687443694E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>64</v>
       </c>
@@ -12996,7 +13185,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>67</v>
       </c>
@@ -13025,7 +13214,7 @@
         <v>8.9992774458843572E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>68</v>
       </c>
@@ -13054,7 +13243,7 @@
         <v>0.105</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>8</v>
       </c>
@@ -13083,7 +13272,7 @@
         <v>8.5001302866310982E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G90" s="4" t="s">
         <v>73</v>
       </c>
@@ -13092,7 +13281,7 @@
         <v>9.3331359108384845E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="17"/>
       <c r="G91" s="4" t="s">
         <v>74</v>
@@ -13102,10 +13291,10 @@
         <v>9.2499447176296073E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="17"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>62</v>
       </c>
@@ -13125,7 +13314,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>1</v>
       </c>
@@ -13150,7 +13339,7 @@
         <v>2195.2919997265985</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>2</v>
       </c>
@@ -13175,7 +13364,7 @@
         <v>2095.3508539406994</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>3</v>
       </c>
@@ -13200,7 +13389,7 @@
         <v>1999.9595505549189</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>4</v>
       </c>
@@ -13225,7 +13414,7 @@
         <v>1908.9109570043559</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>5</v>
       </c>
@@ -13250,7 +13439,7 @@
         <v>1822.0073704791771</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>6</v>
       </c>
@@ -13275,7 +13464,7 @@
         <v>24422.452549063033</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>7</v>
       </c>
@@ -13297,7 +13486,7 @@
         <v>1010.3672172906821</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>8</v>
       </c>
@@ -13319,7 +13508,7 @@
         <v>964.37002995837429</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>9</v>
       </c>
@@ -13341,7 +13530,7 @@
         <v>920.46687458422582</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>10</v>
       </c>
@@ -13363,7 +13552,7 @@
         <v>7154.0082763926421</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>11</v>
       </c>
@@ -13382,7 +13571,7 @@
         <v>628.92425598397301</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>12</v>
       </c>
@@ -13401,7 +13590,7 @@
         <v>600.29234243287806</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>13</v>
       </c>
@@ -13420,7 +13609,7 @@
         <v>572.96390297392918</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>14</v>
       </c>
@@ -13439,7 +13628,7 @@
         <v>10963.633818866752</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E109" s="4" t="s">
         <v>9</v>
       </c>
@@ -13448,7 +13637,7 @@
         <v>57258.999999252228</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E110" s="4" t="s">
         <v>81</v>
       </c>
@@ -13457,22 +13646,22 @@
         <v>7.4777199188247323E-7</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>14</v>
       </c>
@@ -13480,7 +13669,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>15</v>
       </c>
@@ -13488,7 +13677,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>17</v>
       </c>
@@ -13496,7 +13685,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>46</v>
       </c>
@@ -13504,7 +13693,7 @@
         <v>769.4</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>16</v>
       </c>
@@ -13512,7 +13701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>72</v>
       </c>
@@ -13520,7 +13709,7 @@
         <v>0.10000207709700132</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="11" t="s">
         <v>87</v>
       </c>
@@ -13528,7 +13717,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="11" t="s">
         <v>88</v>
       </c>
@@ -13536,7 +13725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>42</v>
       </c>
@@ -13559,7 +13748,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="22" cm="1">
         <f t="array" ref="A128:A157">_xlfn.SEQUENCE($B$119*$B$122, 1, 1)</f>
         <v>1</v>
@@ -13589,7 +13778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>2</v>
       </c>
@@ -13618,7 +13807,7 @@
         <v>1.63287734065189E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>3</v>
       </c>
@@ -13647,7 +13836,7 @@
         <v>4.8071979383408799E-3</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>4</v>
       </c>
@@ -13676,7 +13865,7 @@
         <v>9.4317803769967366E-3</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>5</v>
       </c>
@@ -13705,7 +13894,7 @@
         <v>1.5416066357058096E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>6</v>
       </c>
@@ -13734,7 +13923,7 @@
         <v>2.2670467461765827E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>7</v>
       </c>
@@ -13763,7 +13952,7 @@
         <v>3.1106686641078251E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>8</v>
       </c>
@@ -13792,7 +13981,7 @@
         <v>4.0638013223662485E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>9</v>
       </c>
@@ -13821,7 +14010,7 @@
         <v>5.1179590661895875E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>10</v>
       </c>
@@ -13850,7 +14039,7 @@
         <v>6.2648656587786969E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>11</v>
       </c>
@@ -13879,7 +14068,7 @@
         <v>7.4964755104453176E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>12</v>
       </c>
@@ -13908,7 +14097,7 @@
         <v>8.8049921554582619E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>13</v>
       </c>
@@ -13937,7 +14126,7 @@
         <v>0.10182884029154343</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>14</v>
       </c>
@@ -13966,7 +14155,7 @@
         <v>0.11622897622883752</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>15</v>
       </c>
@@ -13995,7 +14184,7 @@
         <v>0.13118068115869816</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>16</v>
       </c>
@@ -14024,7 +14213,7 @@
         <v>0.14661727601089675</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <v>17</v>
       </c>
@@ -14053,7 +14242,7 @@
         <v>0.16247511036903431</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
         <v>18</v>
       </c>
@@ -14082,7 +14271,7 @@
         <v>0.17869360067516102</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>19</v>
       </c>
@@ -14111,7 +14300,7 @@
         <v>0.19521524863634898</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>20</v>
       </c>
@@ -14140,7 +14329,7 @@
         <v>0.21198564140110573</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>21</v>
       </c>
@@ -14169,7 +14358,7 @@
         <v>0.22895343510176897</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>22</v>
       </c>
@@ -14198,7 +14387,7 @@
         <v>0.24607032336396273</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>23</v>
       </c>
@@ -14227,7 +14416,7 @@
         <v>0.26329099236860132</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>24</v>
       </c>
@@ -14256,7 +14445,7 @@
         <v>0.28057306401858401</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>25</v>
       </c>
@@ -14285,7 +14474,7 @@
         <v>0.29787702871398031</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>26</v>
       </c>
@@ -14314,7 +14503,7 @@
         <v>0.31516616917877993</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>27</v>
       </c>
@@ -14343,7 +14532,7 @@
         <v>0.33240647671167867</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>28</v>
       </c>
@@ -14372,7 +14561,7 @@
         <v>0.34956656115518586</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
         <v>29</v>
       </c>
@@ -14401,7 +14590,7 @@
         <v>0.36661755579370092</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>30</v>
       </c>
@@ -14430,7 +14619,7 @@
         <v>0.38353301830400366</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B159" s="4" t="s">
         <v>9</v>
       </c>
@@ -14443,7 +14632,7 @@
         <v>769.39999954944017</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B160" s="4" t="s">
         <v>90</v>
       </c>
@@ -14453,7 +14642,7 @@
       </c>
       <c r="D160" s="3"/>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C162" t="s">
         <v>91</v>
       </c>
@@ -14462,12 +14651,12 @@
         <v>4.5055980990582611E-7</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>83</v>
       </c>
@@ -14481,12 +14670,275 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02679EC0-6371-4C77-A0D4-51EADCAF875A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9">
+        <v>0.04</v>
+      </c>
+      <c r="C9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <f>$B$7*A13</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="25">
+        <f>-PV($B$9, $B$10, B13, $B$7)</f>
+        <v>45.638694620129208</v>
+      </c>
+      <c r="D13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:B23" si="0">$B$7*A14</f>
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="25">
+        <f t="shared" ref="C14:C23" si="1">-PV($B$9, $B$10, B14, $B$7)</f>
+        <v>52.433857792613054</v>
+      </c>
+      <c r="D14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.01</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C15" s="25">
+        <f t="shared" si="1"/>
+        <v>59.229020965096908</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="C16" s="25">
+        <f t="shared" si="1"/>
+        <v>66.024184137580747</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.02</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C17" s="25">
+        <f t="shared" si="1"/>
+        <v>72.819347310064614</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="C18" s="25">
+        <f t="shared" si="1"/>
+        <v>79.61451048254844</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.03</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C19" s="25">
+        <f t="shared" si="1"/>
+        <v>86.409673655032293</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>3.5000000000000004</v>
+      </c>
+      <c r="C20" s="25">
+        <f t="shared" si="1"/>
+        <v>93.204836827516147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.04</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C21" s="25">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="C22" s="25">
+        <f t="shared" si="1"/>
+        <v>106.79516317248384</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.05</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C23" s="25">
+        <f t="shared" si="1"/>
+        <v>113.59032634496769</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30">
+        <f>$B$7/(1+$B$9)^($B$10)</f>
+        <v>45.638694620129208</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31">
+        <f>$B$10/(1+$B$9)</f>
+        <v>19.23076923076923</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B32">
+        <f>$B$10</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[BAF510] : Add accrued interest date calculation
</commit_message>
<xml_diff>
--- a/BAF510채권/BOND_FINAL_PREP.xlsx
+++ b/BAF510채권/BOND_FINAL_PREP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VSCodeProjects\KAIST_MFE\BAF510채권\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200D2A5C-9D17-40CB-BECC-738BA11FED6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CFFF87-018E-47E6-A0DB-4D9C8299BA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-6945" windowWidth="16440" windowHeight="28440" activeTab="3" xr2:uid="{C3082CC5-84DE-479A-9159-2F50C75C6A87}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C3082CC5-84DE-479A-9159-2F50C75C6A87}"/>
   </bookViews>
   <sheets>
     <sheet name="price" sheetId="1" r:id="rId1"/>
@@ -476,7 +476,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="116">
   <si>
     <t>PV/FV calculator</t>
   </si>
@@ -809,6 +809,21 @@
   </si>
   <si>
     <t xml:space="preserve">엑셀에 있음. </t>
+  </si>
+  <si>
+    <t>coupon date t-1</t>
+  </si>
+  <si>
+    <t>coupon date t</t>
+  </si>
+  <si>
+    <t>today</t>
+  </si>
+  <si>
+    <t>t-1 diff</t>
+  </si>
+  <si>
+    <t>[t-1~today] / [t-1 ~ t]</t>
   </si>
 </sst>
 </file>
@@ -8380,10 +8395,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2340D6-5A21-4368-AD7B-2B859CA61B98}">
-  <dimension ref="A1:H116"/>
+  <dimension ref="A1:L116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8395,30 +8410,63 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K2" s="17">
+        <v>45214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K3" s="17">
+        <v>45327</v>
+      </c>
+      <c r="L3">
+        <f>K3-$K$2</f>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K4" s="17">
+        <v>45397</v>
+      </c>
+      <c r="L4">
+        <f>K4-$K$2</f>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
@@ -8426,7 +8474,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -8434,7 +8482,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>32</v>
       </c>
@@ -8442,7 +8490,16 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>115</v>
+      </c>
+      <c r="K8">
+        <f>$L$3/$L$4</f>
+        <v>0.61748633879781423</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -8451,7 +8508,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -8460,7 +8517,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -8469,7 +8526,7 @@
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -8478,7 +8535,7 @@
         <v>597.51912424641466</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>34</v>
       </c>
@@ -8487,7 +8544,7 @@
         <v>342.72896332894379</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
@@ -8496,7 +8553,7 @@
         <v>940.24808757535845</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>35</v>
       </c>
@@ -8827,7 +8884,7 @@
         <v>983.18496232084067</v>
       </c>
       <c r="G26" s="7">
-        <f t="shared" si="5"/>
+        <f>$B$9*(1-B26)</f>
         <v>39.99999999999968</v>
       </c>
       <c r="H26" s="7">
@@ -8997,7 +9054,7 @@
         <v>985.07197682807214</v>
       </c>
       <c r="G31" s="7">
-        <f t="shared" si="5"/>
+        <f>$B$9*(1-B31)</f>
         <v>39.999999999999503</v>
       </c>
       <c r="H31" s="7">
@@ -14672,7 +14729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02679EC0-6371-4C77-A0D4-51EADCAF875A}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>

</xml_diff>